<commit_message>
Modify The Database Connection Parameter
</commit_message>
<xml_diff>
--- a/DatabaseHandler/DatabaseDataEntry/BoT_Catalouge_Details.xlsx
+++ b/DatabaseHandler/DatabaseDataEntry/BoT_Catalouge_Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/soumalya_mondal_capgemini_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soumamon\OneDrive - Capgemini\PRiSM-Analytics-Deployment\Azure-Market-Place\DatabaseHandler\DatabaseDataEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6071ACC9-499E-4D4A-B904-0271D667959A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A46BA0-2E59-4CED-85C5-761D26C92611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B0CF95E-3385-44B8-9137-8982B2C8D9C4}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{8B0CF95E-3385-44B8-9137-8982B2C8D9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -8937,6 +8937,21 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="205.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -49449,4 +49464,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{bb5d96ea-ab39-44a0-a6d6-b6f0aac5958b}" enabled="1" method="Privileged" siteId="{76a2ae5a-9f00-4f6b-95ed-5d33d77c4d61}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>